<commit_message>
another tests for rates
</commit_message>
<xml_diff>
--- a/billing/in/rates.xlsx
+++ b/billing/in/rates.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,13 +441,43 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>A200</t>
         </is>
       </c>
       <c r="B2" t="n">
+        <v>150</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>10005</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>A200</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>90</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ALL</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>B300</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>50</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>ALL</t>
         </is>

</xml_diff>

<commit_message>
test the test file
</commit_message>
<xml_diff>
--- a/billing/in/rates.xlsx
+++ b/billing/in/rates.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,43 +441,13 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>A200</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="C2" t="inlineStr">
-        <is>
-          <t>10005</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>A200</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>90</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>ALL</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>B300</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>50</v>
-      </c>
-      <c r="C4" t="inlineStr">
         <is>
           <t>ALL</t>
         </is>

</xml_diff>

<commit_message>
add bill-ui and also did test
</commit_message>
<xml_diff>
--- a/billing/in/rates.xlsx
+++ b/billing/in/rates.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,15 +441,180 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>nnnnn</t>
+          <t>Blood</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4444</v>
+        <v>112</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ALL</t>
+          <t>All</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Clementine</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>113</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Grapefruit</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>88</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Mandarin</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>102</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Mandarin</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>120</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Mandarin</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>104</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Navel</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>93</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Shamuti</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>84</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Tangerine</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>85</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Tangerine</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>92</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>90</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>87</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>All</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update error message in rates and test
</commit_message>
<xml_diff>
--- a/billing/in/rates.xlsx
+++ b/billing/in/rates.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,163 +456,13 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Clementine</t>
+          <t>Navel</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="C3" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Grapefruit</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>88</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Mandarin</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>102</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>43</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Mandarin</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>120</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Mandarin</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>104</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Navel</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>93</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Shamuti</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>84</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Tangerine</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>85</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Tangerine</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>92</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Valencia</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>90</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Valencia</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>87</v>
-      </c>
-      <c r="C13" t="inlineStr">
         <is>
           <t>All</t>
         </is>

</xml_diff>